<commit_message>
Consultation resulta candiat + accueil
</commit_message>
<xml_diff>
--- a/Suivi.xlsx
+++ b/Suivi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Paramètres à renseigner avant d'exploiter l'onglet de suivi</t>
   </si>
@@ -156,6 +156,9 @@
     <t>      – Sélectionner un épreuve</t>
   </si>
   <si>
+    <t>sly</t>
+  </si>
+  <si>
     <t>      – Tirer au sort les questions</t>
   </si>
   <si>
@@ -175,6 +178,9 @@
   </si>
   <si>
     <t>-Reprendre un TEST</t>
+  </si>
+  <si>
+    <t>-Creation Test/Questions</t>
   </si>
   <si>
     <t>Charge estimée/temps passé</t>
@@ -189,7 +195,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="S&quot;tan&quot;D\aRD"/>
+    <numFmt numFmtId="165" formatCode="S&quot;tanJa&quot;R\J"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -612,7 +618,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -740,10 +746,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>134</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -913,11 +919,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="17970234"/>
-        <c:axId val="88543158"/>
+        <c:axId val="94541948"/>
+        <c:axId val="10951028"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17970234"/>
+        <c:axId val="94541948"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,14 +954,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88543158"/>
+        <c:crossAx val="10951028"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88543158"/>
+        <c:axId val="10951028"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +977,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="StanJaRJ" sourceLinked="0"/>
+        <c:numFmt formatCode="S&quot;tanJa&quot;R&quot;J&quot;" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -996,7 +1002,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17970234"/>
+        <c:crossAx val="94541948"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1040,15 +1046,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>72360</xdr:colOff>
+      <xdr:colOff>99000</xdr:colOff>
       <xdr:row>104</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>162360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1056,8 +1062,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="787320" y="13515120"/>
-        <a:ext cx="8085960" cy="5676120"/>
+        <a:off x="804600" y="13506120"/>
+        <a:ext cx="7981200" cy="5675760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1083,12 +1089,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="64.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1193,19 +1199,19 @@
   </sheetPr>
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="13" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.1938775510204"/>
     <col collapsed="false" hidden="true" max="4" min="4" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,12 +1953,12 @@
         <v>43</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="27"/>
       <c r="F30" s="22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
@@ -1970,15 +1976,15 @@
         <v>37</v>
       </c>
       <c r="B31" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="25" t="s">
         <v>44</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>5</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="27"/>
       <c r="F31" s="22" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
@@ -1996,7 +2002,7 @@
         <v>38</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>3</v>
@@ -2020,7 +2026,7 @@
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="21"/>
       <c r="B33" s="26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>3</v>
@@ -2044,10 +2050,10 @@
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="21"/>
       <c r="B34" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="27"/>
@@ -2068,10 +2074,10 @@
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="21"/>
       <c r="B35" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="25" t="s">
         <v>49</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>48</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="27"/>
@@ -2094,10 +2100,10 @@
         <v>39</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="27"/>
@@ -2119,42 +2125,46 @@
       <c r="A37" s="17" t="n">
         <v>40</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
+      <c r="B37" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>5</v>
+      </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P37" s="20" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,18 +2269,18 @@
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="29" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C43" s="29"/>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
       <c r="F43" s="29" t="n">
         <f aca="false">SUM(F7:F42)</f>
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="G43" s="29" t="n">
         <f aca="false">SUM(G8:G42)</f>
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="H43" s="29" t="n">
         <f aca="false">SUM(H42:H42)</f>
@@ -2311,7 +2321,7 @@
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
@@ -2388,7 +2398,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>